<commit_message>
PROS-7547 SANOFIHK Kpi Update
</commit_message>
<xml_diff>
--- a/Projects/SANOFIHK/Data/Template.xlsx
+++ b/Projects/SANOFIHK/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -624,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="76">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -737,6 +737,18 @@
     <t xml:space="preserve">GBD -HK GT Medicine</t>
   </si>
   <si>
+    <t xml:space="preserve">GBD -HK GT TRAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBD -HK GT Store A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBD -HK GT Store B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBD -Macau GT TRAX</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESSENTIALE 60 Capsules</t>
   </si>
   <si>
@@ -764,37 +776,93 @@
     <t xml:space="preserve">Feminine Care</t>
   </si>
   <si>
-    <t xml:space="preserve">LACTACYD FRESH</t>
+    <t xml:space="preserve">Surulac 40 Tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4891609560080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surulac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LACTACYD ADC 250ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8934638030028 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lactacyd ADF 250ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4891609992300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobliity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7891058003968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrition</t>
   </si>
   <si>
     <t xml:space="preserve">SKUs</t>
   </si>
   <si>
-    <t xml:space="preserve">Display Rack_Essentiale_Dulcolax</t>
+    <t xml:space="preserve">Display Rack_Essentiale</t>
   </si>
   <si>
     <t xml:space="preserve">POSM_001</t>
   </si>
   <si>
-    <t xml:space="preserve">Essentiale &amp; Dulcolax</t>
+    <t xml:space="preserve">Display Rack_Surulac &amp; Dulcolax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSM_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surulac &amp; Dulcolax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Box_Mobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSM_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobility</t>
   </si>
   <si>
     <t xml:space="preserve">Lactacyd shelf strip</t>
   </si>
   <si>
-    <t xml:space="preserve">POSM_002</t>
+    <t xml:space="preserve">POSM_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSM_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DULCOLAX 100 Tablets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DULCOLAX 30 Tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surulac 40 Tablets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LACTACYD EP 250ml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0;[RED]0"/>
-    <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -820,18 +888,18 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="177"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="177"/>
     </font>
     <font>
       <b val="true"/>
@@ -940,7 +1008,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -962,7 +1030,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C7E7"/>
-        <bgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FFC5E0B4"/>
       </patternFill>
     </fill>
     <fill>
@@ -986,13 +1054,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE699"/>
-        <bgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFF8CBAD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
-        <bgColor rgb="FFDAE3F3"/>
+        <bgColor rgb="FFA9D18E"/>
       </patternFill>
     </fill>
     <fill>
@@ -1005,6 +1073,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor rgb="FFFFE699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor rgb="FFDAE3F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -1038,7 +1124,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1062,21 +1148,29 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1128,7 +1222,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1136,11 +1230,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1156,42 +1254,34 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1216,7 +1306,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1228,19 +1318,55 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1256,43 +1382,41 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="13" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="20" fillId="14" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="14" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="14" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Explanatory Text 2" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="22" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1332,10 +1456,10 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFC5E0B4"/>
       <rgbColor rgb="FFFFE699"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFA9D18E"/>
+      <rgbColor rgb="FFFFCCFF"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFF8CBAD"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1364,19 +1488,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1632,20 +1756,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="13" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.89068825910931"/>
   </cols>
@@ -1661,7 +1785,7 @@
       </c>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="58.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -1683,231 +1807,316 @@
       <c r="G2" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="H2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="21" t="n">
+      <c r="B3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="22" t="n">
         <v>4891609702053</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="D3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="21" t="n">
+      <c r="B4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="22" t="n">
         <v>4891612591514</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="D4" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="21" t="n">
+      <c r="B5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="22" t="n">
         <v>4891612591521</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
+      <c r="D5" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="22" t="n">
+        <v>4891609810000</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="21" t="n">
-        <v>4891609810000</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="F7" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="21" t="n">
-        <v>4891609040032</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="B8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="B9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
-      <c r="B15" s="26"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="22"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="22"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="22"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-    </row>
+      <c r="B10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AMJ10" s="0"/>
+    </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
@@ -1930,26 +2139,26 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
-    <row r="1" s="28" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="16" t="s">
         <v>30</v>
       </c>
@@ -1966,7 +2175,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>32</v>
@@ -1977,136 +2186,136 @@
       <c r="G2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="29"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2130,27 +2339,27 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="35" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="35" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="36" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="35" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="16" t="s">
         <v>30</v>
       </c>
@@ -2199,21 +2408,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="38" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="38" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="38" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2223,113 +2432,250 @@
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="39"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="39" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
+      <c r="H2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="E6" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="43" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43" t="s">
+      <c r="F6" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="43" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
+      <c r="B7" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2351,198 +2697,355 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:AMI10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="16" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="40" t="s">
+    <row r="2" customFormat="false" ht="58.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="39" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
+      <c r="H2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="48" t="n">
+      <c r="B3" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="55" t="n">
         <v>4891609702053</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="50" t="n">
+      <c r="D3" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="56" t="n">
         <v>3</v>
       </c>
-      <c r="G3" s="50" t="n">
+      <c r="I3" s="56" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="s">
+      <c r="J3" s="56" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" s="56" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="48" t="n">
+      <c r="B4" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="55" t="n">
         <v>4891612591514</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="50" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="50" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="s">
+      <c r="D4" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="56" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="55" t="n">
+        <v>4891612591514</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AMI5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="55" t="n">
+        <v>4891612591514</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMI6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMI7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="E8" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="50" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="53"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="53"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="53"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="53"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="53"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="53"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="53"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="53"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="53"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F8" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMI8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMI9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMI10" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
SanofiHK Template Change - Only updated POSM facings
</commit_message>
<xml_diff>
--- a/Projects/SANOFIHK/Data/Template.xlsx
+++ b/Projects/SANOFIHK/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -1127,7 +1127,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1151,16 +1151,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1221,7 +1217,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1229,11 +1225,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1253,7 +1249,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1261,7 +1257,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="14" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1305,7 +1301,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1317,11 +1313,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1385,10 +1381,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1405,7 +1397,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1413,20 +1405,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1502,9 +1493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971440</xdr:colOff>
+      <xdr:colOff>2971080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1514,7 +1505,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8800560" cy="6349320"/>
+          <a:ext cx="8838360" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1547,9 +1538,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971440</xdr:colOff>
+      <xdr:colOff>2971080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1559,7 +1550,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8800560" cy="6349320"/>
+          <a:ext cx="8838360" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1592,9 +1583,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971440</xdr:colOff>
+      <xdr:colOff>2971080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1604,7 +1595,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8800560" cy="6349320"/>
+          <a:ext cx="8838360" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1637,9 +1628,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971440</xdr:colOff>
+      <xdr:colOff>2971080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1649,7 +1640,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8800560" cy="6349320"/>
+          <a:ext cx="8838360" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1682,9 +1673,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971440</xdr:colOff>
+      <xdr:colOff>2971080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1694,7 +1685,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8800560" cy="6349320"/>
+          <a:ext cx="8838360" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1727,9 +1718,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971440</xdr:colOff>
+      <xdr:colOff>2971080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1739,7 +1730,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8800560" cy="6349320"/>
+          <a:ext cx="8838360" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1777,9 +1768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523520</xdr:colOff>
+      <xdr:colOff>1523160</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1789,7 +1780,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7714440" cy="6349320"/>
+          <a:ext cx="7761960" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1822,9 +1813,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523520</xdr:colOff>
+      <xdr:colOff>1523160</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1834,7 +1825,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7714440" cy="6349320"/>
+          <a:ext cx="7761960" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1867,9 +1858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523520</xdr:colOff>
+      <xdr:colOff>1523160</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1879,7 +1870,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7714440" cy="6349320"/>
+          <a:ext cx="7761960" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1912,9 +1903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523520</xdr:colOff>
+      <xdr:colOff>1523160</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1924,7 +1915,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7714440" cy="6349320"/>
+          <a:ext cx="7761960" cy="6348960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1962,9 +1953,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929960</xdr:colOff>
+      <xdr:colOff>1929600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1974,7 +1965,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7616160" cy="6351480"/>
+          <a:ext cx="7673040" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2007,9 +1998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929960</xdr:colOff>
+      <xdr:colOff>1929600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2019,7 +2010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7616160" cy="6351480"/>
+          <a:ext cx="7673040" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2052,9 +2043,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929960</xdr:colOff>
+      <xdr:colOff>1929600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2064,7 +2055,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7616160" cy="6351480"/>
+          <a:ext cx="7673040" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2097,9 +2088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929960</xdr:colOff>
+      <xdr:colOff>1929600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2109,7 +2100,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7616160" cy="6351480"/>
+          <a:ext cx="7673040" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2142,9 +2133,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929960</xdr:colOff>
+      <xdr:colOff>1929600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2154,7 +2145,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7616160" cy="6351480"/>
+          <a:ext cx="7673040" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2192,9 +2183,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>431280</xdr:colOff>
+      <xdr:colOff>430920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2204,7 +2195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8022600" cy="6352560"/>
+          <a:ext cx="8079480" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2237,9 +2228,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>431280</xdr:colOff>
+      <xdr:colOff>430920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2249,7 +2240,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8022600" cy="6352560"/>
+          <a:ext cx="8079480" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2282,9 +2273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>431280</xdr:colOff>
+      <xdr:colOff>430920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2294,7 +2285,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8022600" cy="6352560"/>
+          <a:ext cx="8079480" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2327,9 +2318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>431280</xdr:colOff>
+      <xdr:colOff>430920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2339,7 +2330,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8022600" cy="6352560"/>
+          <a:ext cx="8079480" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2372,9 +2363,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>431280</xdr:colOff>
+      <xdr:colOff>430920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2384,7 +2375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8022600" cy="6352560"/>
+          <a:ext cx="8079480" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2417,9 +2408,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>431280</xdr:colOff>
+      <xdr:colOff>430920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2429,7 +2420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8022600" cy="6352560"/>
+          <a:ext cx="8079480" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2467,9 +2458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1041120</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2479,7 +2470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7851240" cy="6351480"/>
+          <a:ext cx="7898760" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2512,9 +2503,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1041120</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2524,7 +2515,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7851240" cy="6351480"/>
+          <a:ext cx="7898760" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2557,9 +2548,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1041120</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2569,7 +2560,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7851240" cy="6351480"/>
+          <a:ext cx="7898760" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2602,9 +2593,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1041120</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2614,7 +2605,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7851240" cy="6351480"/>
+          <a:ext cx="7898760" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2647,9 +2638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1041120</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2659,7 +2650,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7851240" cy="6351480"/>
+          <a:ext cx="7898760" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2692,9 +2683,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1041120</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2704,7 +2695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7851240" cy="6351480"/>
+          <a:ext cx="7898760" cy="6351120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2744,13 +2735,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3008,18 +2999,18 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="13" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
   </cols>
@@ -3396,11 +3387,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3608,11 +3599,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="38.3481781376518"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="35" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
@@ -3690,19 +3681,19 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="29.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3823,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3928,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3978,7 +3969,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
@@ -3986,12 +3977,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1022" min="8" style="14" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
   </cols>
@@ -4068,16 +4059,16 @@
       <c r="G3" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="56" t="n">
+      <c r="H3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="56" t="n">
+      <c r="I3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="56" t="n">
+      <c r="J3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="K3" s="56" t="n">
+      <c r="K3" s="14" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4103,16 +4094,16 @@
       <c r="G4" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="56" t="n">
+      <c r="H4" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="14" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4138,16 +4129,16 @@
       <c r="G5" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="56" t="n">
+      <c r="H5" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="56" t="n">
+      <c r="I5" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="J5" s="56" t="n">
+      <c r="J5" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="K5" s="56" t="n">
+      <c r="K5" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4173,16 +4164,16 @@
       <c r="G6" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="56" t="n">
+      <c r="H6" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="14" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4208,33 +4199,33 @@
       <c r="G7" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="56" t="n">
+      <c r="H7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="I7" s="56" t="n">
+      <c r="I7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="56" t="n">
+      <c r="J7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="K7" s="56" t="n">
+      <c r="K7" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="59" t="n">
+      <c r="C8" s="58" t="n">
         <v>4891609810000</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="59" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="50" t="n">
@@ -4243,33 +4234,33 @@
       <c r="G8" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="56" t="n">
+      <c r="H8" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="56" t="n">
+      <c r="I8" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="56" t="n">
+      <c r="J8" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="56" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="59" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="50" t="n">
@@ -4278,33 +4269,33 @@
       <c r="G9" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="56" t="n">
+      <c r="H9" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="56" t="n">
+      <c r="I9" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="J9" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="56" t="n">
+      <c r="J9" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="59" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="50" t="n">
@@ -4313,21 +4304,18 @@
       <c r="G10" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="56" t="n">
+      <c r="H10" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="I10" s="56" t="n">
+      <c r="I10" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="J10" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="56" t="n">
+      <c r="J10" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="14" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
SanofiHK Template Change - Updated Ean code for DUCOLAX 100 Tablets in Primary&Secondary facings tab according to PROS-8114
</commit_message>
<xml_diff>
--- a/Projects/SANOFIHK/Data/Template.xlsx
+++ b/Projects/SANOFIHK/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -1493,9 +1493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971080</xdr:colOff>
+      <xdr:colOff>2970720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1505,7 +1505,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8838360" cy="6348960"/>
+          <a:ext cx="8885520" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1538,9 +1538,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971080</xdr:colOff>
+      <xdr:colOff>2970720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1550,7 +1550,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8838360" cy="6348960"/>
+          <a:ext cx="8885520" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1583,9 +1583,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971080</xdr:colOff>
+      <xdr:colOff>2970720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1595,7 +1595,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8838360" cy="6348960"/>
+          <a:ext cx="8885520" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1628,9 +1628,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971080</xdr:colOff>
+      <xdr:colOff>2970720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1640,7 +1640,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8838360" cy="6348960"/>
+          <a:ext cx="8885520" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1673,9 +1673,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971080</xdr:colOff>
+      <xdr:colOff>2970720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1685,7 +1685,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8838360" cy="6348960"/>
+          <a:ext cx="8885520" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1718,9 +1718,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2971080</xdr:colOff>
+      <xdr:colOff>2970720</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1730,7 +1730,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8838360" cy="6348960"/>
+          <a:ext cx="8885520" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1768,9 +1768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523160</xdr:colOff>
+      <xdr:colOff>1522800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1780,7 +1780,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7761960" cy="6348960"/>
+          <a:ext cx="7809120" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1813,9 +1813,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523160</xdr:colOff>
+      <xdr:colOff>1522800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1825,7 +1825,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7761960" cy="6348960"/>
+          <a:ext cx="7809120" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1858,9 +1858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523160</xdr:colOff>
+      <xdr:colOff>1522800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1870,7 +1870,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7761960" cy="6348960"/>
+          <a:ext cx="7809120" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1903,9 +1903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1523160</xdr:colOff>
+      <xdr:colOff>1522800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1915,7 +1915,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7761960" cy="6348960"/>
+          <a:ext cx="7809120" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1953,9 +1953,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929600</xdr:colOff>
+      <xdr:colOff>1929240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1965,7 +1965,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7673040" cy="6351120"/>
+          <a:ext cx="7729920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1998,9 +1998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929600</xdr:colOff>
+      <xdr:colOff>1929240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2010,7 +2010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7673040" cy="6351120"/>
+          <a:ext cx="7729920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2043,9 +2043,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929600</xdr:colOff>
+      <xdr:colOff>1929240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2055,7 +2055,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7673040" cy="6351120"/>
+          <a:ext cx="7729920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2088,9 +2088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929600</xdr:colOff>
+      <xdr:colOff>1929240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2100,7 +2100,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7673040" cy="6351120"/>
+          <a:ext cx="7729920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2133,9 +2133,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1929600</xdr:colOff>
+      <xdr:colOff>1929240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2145,7 +2145,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7673040" cy="6351120"/>
+          <a:ext cx="7729920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2183,9 +2183,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>430920</xdr:colOff>
+      <xdr:colOff>430560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2195,7 +2195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8079480" cy="6352200"/>
+          <a:ext cx="8136000" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2228,9 +2228,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>430920</xdr:colOff>
+      <xdr:colOff>430560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2240,7 +2240,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8079480" cy="6352200"/>
+          <a:ext cx="8136000" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2273,9 +2273,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>430920</xdr:colOff>
+      <xdr:colOff>430560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2285,7 +2285,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8079480" cy="6352200"/>
+          <a:ext cx="8136000" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2318,9 +2318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>430920</xdr:colOff>
+      <xdr:colOff>430560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2330,7 +2330,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8079480" cy="6352200"/>
+          <a:ext cx="8136000" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2363,9 +2363,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>430920</xdr:colOff>
+      <xdr:colOff>430560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2375,7 +2375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8079480" cy="6352200"/>
+          <a:ext cx="8136000" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2408,9 +2408,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>430920</xdr:colOff>
+      <xdr:colOff>430560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2420,7 +2420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8079480" cy="6352200"/>
+          <a:ext cx="8136000" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2458,9 +2458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1040760</xdr:colOff>
+      <xdr:colOff>1040400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2470,7 +2470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7898760" cy="6351120"/>
+          <a:ext cx="7945920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2503,9 +2503,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1040760</xdr:colOff>
+      <xdr:colOff>1040400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2515,7 +2515,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7898760" cy="6351120"/>
+          <a:ext cx="7945920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2548,9 +2548,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1040760</xdr:colOff>
+      <xdr:colOff>1040400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2560,7 +2560,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7898760" cy="6351120"/>
+          <a:ext cx="7945920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2593,9 +2593,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1040760</xdr:colOff>
+      <xdr:colOff>1040400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2605,7 +2605,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7898760" cy="6351120"/>
+          <a:ext cx="7945920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2638,9 +2638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1040760</xdr:colOff>
+      <xdr:colOff>1040400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2650,7 +2650,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7898760" cy="6351120"/>
+          <a:ext cx="7945920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2683,9 +2683,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1040760</xdr:colOff>
+      <xdr:colOff>1040400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2695,7 +2695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7898760" cy="6351120"/>
+          <a:ext cx="7945920" cy="6350760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2735,13 +2735,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3005,12 +3005,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="13" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
   </cols>
@@ -3387,11 +3387,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3599,11 +3599,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="35" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
@@ -3681,18 +3681,18 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="29.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="14" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
   </cols>
@@ -3971,18 +3971,18 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.8825910931174"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="45.2024291497976"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1022" min="8" style="14" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
   </cols>
@@ -4115,7 +4115,7 @@
         <v>70</v>
       </c>
       <c r="C5" s="55" t="n">
-        <v>4891612591514</v>
+        <v>4891612591521</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>45</v>

</xml_diff>